<commit_message>
Login screen done I think
</commit_message>
<xml_diff>
--- a/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
+++ b/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misae\IdeaProjects\java-4thsemester\ProyectoFarmacia\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FE11E5-65DB-4672-8E21-DB12211DD707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B478A7A-FD10-4445-9188-B618C737898F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Folio</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Stock</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>6005</t>
   </si>
   <si>
@@ -93,13 +90,18 @@
   </si>
   <si>
     <t>Medicina</t>
+  </si>
+  <si>
+    <t>3881</t>
+  </si>
+  <si>
+    <t>Talco para bebé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,12 +421,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -454,18 +456,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DC127B-7FA2-4E73-B844-D1876EA0262F}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D10" sqref="A9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="42.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,39 +533,53 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5.0</v>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Practica 3 Unidad 2
</commit_message>
<xml_diff>
--- a/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
+++ b/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Folio</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>Stock</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>6771</t>
+  </si>
+  <si>
+    <t>Aspirina 250mg</t>
+  </si>
+  <si>
+    <t>Talco para pies</t>
   </si>
 </sst>
 </file>
@@ -511,7 +523,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DC127B-7FA2-4E73-B844-D1876EA0262F}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
@@ -550,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,8 +575,8 @@
       <c r="C3">
         <v>40</v>
       </c>
-      <c r="D3">
-        <v>7</v>
+      <c r="D3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,7 +604,7 @@
         <v>36</v>
       </c>
       <c r="D5" t="n">
-        <v>28.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,13 +626,13 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="C7" t="n">
+        <v>25.0</v>
       </c>
       <c r="D7" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,7 +660,7 @@
         <v>134</v>
       </c>
       <c r="D9" t="n">
-        <v>17.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,100 +679,86 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C11">
-        <v>89</v>
+        <v>332</v>
       </c>
       <c r="D11" t="n">
-        <v>7.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C12">
-        <v>1122</v>
-      </c>
-      <c r="D12" t="n">
-        <v>6.0</v>
+        <v>113</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C13">
-        <v>332</v>
-      </c>
-      <c r="D13">
-        <v>18</v>
+        <v>96</v>
+      </c>
+      <c r="D13" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14">
-        <v>113</v>
-      </c>
-      <c r="D14">
-        <v>40</v>
+        <v>579</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C15">
-        <v>96</v>
-      </c>
-      <c r="D15" t="n">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+      <c r="D15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>579</v>
+        <v>43</v>
+      </c>
+      <c r="C16" t="n">
+        <v>35.0</v>
       </c>
       <c r="D16" t="n">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17">
-        <v>449</v>
-      </c>
-      <c r="D17">
-        <v>18</v>
+        <v>20.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Practica 5 Unidad 2
</commit_message>
<xml_diff>
--- a/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
+++ b/ProyectoFarmacia/src/resources/vesa_pharmacy.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>Folio</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Vick 44 90ml</t>
+  </si>
+  <si>
+    <t>Fabe Naproxeno Paracetamol 10 tabletas</t>
   </si>
 </sst>
 </file>
@@ -638,7 +641,7 @@
         <v>102</v>
       </c>
       <c r="D7" t="n">
-        <v>26.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,13 +663,13 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9">
-        <v>70</v>
+        <v>47</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50.0</v>
       </c>
       <c r="D9" t="n">
-        <v>33.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>